<commit_message>
add datos trazabilidad de informes semanales ISCII
</commit_message>
<xml_diff>
--- a/datos/positividad_Ministerio.xlsx
+++ b/datos/positividad_Ministerio.xlsx
@@ -19,8 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Fuente: informe diario Sanidad</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">De informe ISCII</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -29,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Positividad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%Trazabilidad</t>
   </si>
 </sst>
 </file>
@@ -145,15 +184,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -166,6 +205,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -173,6 +215,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -180,6 +223,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -187,6 +231,7 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -194,6 +239,7 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -201,6 +247,7 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -208,6 +255,9 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
+      <c r="D7" s="3" t="n">
+        <v>74.7</v>
+      </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -219,6 +269,7 @@
       <c r="C8" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -230,6 +281,7 @@
       <c r="C9" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -241,6 +293,7 @@
       <c r="C10" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -252,6 +305,7 @@
       <c r="C11" s="3" t="n">
         <v>10.1</v>
       </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -263,6 +317,7 @@
       <c r="C12" s="3" t="n">
         <v>10.5</v>
       </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -270,6 +325,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -277,6 +333,9 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
+      <c r="D14" s="3" t="n">
+        <v>75.3</v>
+      </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -288,6 +347,7 @@
       <c r="C15" s="3" t="n">
         <v>11.7</v>
       </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -299,6 +359,7 @@
       <c r="C16" s="3" t="n">
         <v>12.6</v>
       </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -310,6 +371,7 @@
       <c r="C17" s="3" t="n">
         <v>12.9</v>
       </c>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -321,6 +383,7 @@
       <c r="C18" s="3" t="n">
         <v>12.9</v>
       </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -332,6 +395,7 @@
       <c r="C19" s="0" t="n">
         <v>12.9</v>
       </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -343,6 +407,7 @@
       <c r="C20" s="3" t="n">
         <v>14.7</v>
       </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -350,6 +415,9 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
+      <c r="D21" s="3" t="n">
+        <v>75.9</v>
+      </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -357,6 +425,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -368,6 +437,7 @@
       <c r="C23" s="3" t="n">
         <v>15.2</v>
       </c>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -379,6 +449,7 @@
       <c r="C24" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -390,6 +461,7 @@
       <c r="C25" s="3" t="n">
         <v>16.1</v>
       </c>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -400,6 +472,21 @@
       </c>
       <c r="C26" s="3" t="n">
         <v>16.5</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>44124</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>44125</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>76.2</v>
       </c>
     </row>
   </sheetData>
@@ -410,5 +497,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>